<commit_message>
Se suben cambios en inscrito maestria nueva columnas: correo y cel
</commit_message>
<xml_diff>
--- a/modules/admision/views/inscripcion/files/template_inscritos_maestria.xlsx
+++ b/modules/admision/views/inscripcion/files/template_inscritos_maestria.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="118">
   <si>
     <t>Count of CANTóN</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>SEGUNDO APELLIDO</t>
+  </si>
+  <si>
+    <t>CORREO</t>
+  </si>
+  <si>
+    <t>CELULAR</t>
   </si>
   <si>
     <t>REVISIóN</t>
@@ -376,10 +382,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -465,75 +471,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,7 +493,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -564,9 +531,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -577,8 +565,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,6 +589,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -599,11 +597,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -670,7 +676,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,121 +844,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,49 +856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,17 +922,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -946,6 +946,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -953,6 +977,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,185 +1015,152 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="41" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1583,11 +1589,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" refreshedDate="43696.7703125" refreshedBy="edu" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" refreshedDate="43710.8402314815" refreshedBy="edu" recordCount="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:T1048576" sheet="DATA"/>
+    <worksheetSource ref="A1:V1048576" sheet="DATA"/>
   </cacheSource>
-  <cacheFields count="20">
+  <cacheFields count="22">
     <cacheField name="ID" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNonDate="0" count="1">
         <m/>
@@ -1748,6 +1754,16 @@
         <m/>
       </sharedItems>
     </cacheField>
+    <cacheField name="CORREO" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNonDate="0" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="CELULAR" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNonDate="0" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="REVISIóN" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNonDate="0" count="1">
         <m/>
@@ -1825,6 +1841,8 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1832,7 +1850,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Datos" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="" updatedVersion="5" compact="0" compactData="0" showDrill="1">
   <location ref="A1:D4" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
-  <pivotFields count="20">
+  <pivotFields count="22">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -2003,6 +2021,8 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -2097,7 +2117,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Introd" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="" updatedVersion="5" compact="0" compactData="0" showDrill="1">
   <location ref="A1:C3" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
-  <pivotFields count="20">
+  <pivotFields count="22">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -2238,6 +2258,8 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
@@ -2541,7 +2563,16 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3 C3:D3"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" activeRow="2" previousRow="2" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="3" count="1">
+              <x v="35"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -2611,7 +2642,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="2"/>
@@ -7656,10 +7687,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -7671,18 +7702,20 @@
     <col min="6" max="6" width="47.7142857142857" style="1" customWidth="1"/>
     <col min="7" max="7" width="63.7142857142857" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85714285714286" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7142857142857" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.1428571428571" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="14" width="36.8571428571429" style="1" customWidth="1"/>
-    <col min="15" max="15" width="34" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24.7142857142857" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.14285714285714" style="1"/>
+    <col min="9" max="9" width="20.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7142857142857" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="1" customWidth="1"/>
+    <col min="16" max="16" width="36.8571428571429" style="1" customWidth="1"/>
+    <col min="17" max="17" width="34" style="1" customWidth="1"/>
+    <col min="18" max="18" width="24.7142857142857" style="1" customWidth="1"/>
+    <col min="19" max="21" width="9.14285714285714" style="1"/>
+    <col min="22" max="22" width="18.5714285714286" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:20">
+    <row r="1" s="1" customFormat="1" spans="1:22">
       <c r="A1" s="2" t="s">
         <v>100</v>
       </c>
@@ -7742,6 +7775,12 @@
       </c>
       <c r="T1" s="2" t="s">
         <v>115</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>